<commit_message>
correcting part 3 and 4
</commit_message>
<xml_diff>
--- a/HW2/part_3/results/ec_pdc_20_OUT_size3.xlsx
+++ b/HW2/part_3/results/ec_pdc_20_OUT_size3.xlsx
@@ -37,43 +37,43 @@
     <t>Uniqueness</t>
   </si>
   <si>
-    <t>1064.6+-15.0</t>
-  </si>
-  <si>
-    <t>933.2+-16.6</t>
-  </si>
-  <si>
-    <t>206.7+-9.1</t>
-  </si>
-  <si>
-    <t>1250.3+-14.6</t>
-  </si>
-  <si>
-    <t>304.2+-13.8</t>
-  </si>
-  <si>
-    <t>20.5+-4.6</t>
-  </si>
-  <si>
-    <t>370.3+-12.4</t>
-  </si>
-  <si>
-    <t>27.6+-3.2</t>
-  </si>
-  <si>
-    <t>16.0+-4.2</t>
-  </si>
-  <si>
-    <t>33.7+-5.9</t>
-  </si>
-  <si>
-    <t>59.2+-6.4</t>
-  </si>
-  <si>
-    <t>13.7+-3.0</t>
-  </si>
-  <si>
-    <t>0.6+-0.7</t>
+    <t>561.9+-13.2</t>
+  </si>
+  <si>
+    <t>893.3+-17.1</t>
+  </si>
+  <si>
+    <t>276.0+-10.9</t>
+  </si>
+  <si>
+    <t>1227.1+-13.5</t>
+  </si>
+  <si>
+    <t>222.3+-12.4</t>
+  </si>
+  <si>
+    <t>27.6+-4.7</t>
+  </si>
+  <si>
+    <t>621.6+-14.1</t>
+  </si>
+  <si>
+    <t>89.1+-5.9</t>
+  </si>
+  <si>
+    <t>20.1+-4.4</t>
+  </si>
+  <si>
+    <t>43.0+-6.1</t>
+  </si>
+  <si>
+    <t>61.9+-6.6</t>
+  </si>
+  <si>
+    <t>29.7+-4.6</t>
+  </si>
+  <si>
+    <t>3.7+-1.7</t>
   </si>
 </sst>
 </file>
@@ -468,19 +468,19 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>860</v>
+        <v>346</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2">
-        <v>-13.63</v>
+        <v>-16.3</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>223.14</v>
+        <v>97.68000000000001</v>
       </c>
       <c r="H2">
         <v>14</v>
@@ -494,22 +494,22 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>834</v>
+        <v>799</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
-        <v>-5.97</v>
+        <v>-5.5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>216.4</v>
+        <v>225.58</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -520,22 +520,22 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4">
-        <v>-6.36</v>
+        <v>-8.359999999999999</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>38.66</v>
+        <v>52.23</v>
       </c>
       <c r="H4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -546,19 +546,19 @@
         <v>36</v>
       </c>
       <c r="C5">
-        <v>1076</v>
+        <v>1049</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5">
-        <v>-11.98</v>
+        <v>-13.19</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>279.19</v>
+        <v>296.16</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -572,22 +572,22 @@
         <v>38</v>
       </c>
       <c r="C6">
-        <v>448</v>
+        <v>354</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6">
-        <v>10.41</v>
+        <v>10.64</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>116.24</v>
+        <v>99.94</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -598,22 +598,22 @@
         <v>46</v>
       </c>
       <c r="C7">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7">
-        <v>6.65</v>
+        <v>9.81</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>13.23</v>
+        <v>20.89</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -624,22 +624,22 @@
         <v>74</v>
       </c>
       <c r="C8">
-        <v>252</v>
+        <v>455</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8">
-        <v>-9.57</v>
+        <v>-11.84</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>65.39</v>
+        <v>128.46</v>
       </c>
       <c r="H8">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -650,19 +650,19 @@
         <v>78</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>-4.93</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>3.11</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="H9">
         <v>4</v>
@@ -676,22 +676,22 @@
         <v>98</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10">
-        <v>-2.59</v>
+        <v>-1.84</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0.9740000000000001</v>
       </c>
       <c r="G10">
-        <v>1.3</v>
+        <v>3.39</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -702,22 +702,22 @@
         <v>102</v>
       </c>
       <c r="C11">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11">
-        <v>-1.98</v>
+        <v>-2.12</v>
       </c>
       <c r="F11">
-        <v>0.985</v>
+        <v>0.986</v>
       </c>
       <c r="G11">
-        <v>5.71</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -728,22 +728,22 @@
         <v>108</v>
       </c>
       <c r="C12">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12">
-        <v>9.529999999999999</v>
+        <v>12.68</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>31.14</v>
+        <v>41.22</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -754,19 +754,19 @@
         <v>110</v>
       </c>
       <c r="C13">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13">
-        <v>2.77</v>
+        <v>2.49</v>
       </c>
       <c r="F13">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="G13">
-        <v>5.71</v>
+        <v>11.58</v>
       </c>
       <c r="H13">
         <v>6</v>
@@ -780,22 +780,22 @@
         <v>238</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14">
-        <v>3.38</v>
+        <v>9.23</v>
       </c>
       <c r="F14">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0.78</v>
+        <v>5.36</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>